<commit_message>
Uart Rx verified by test bench.
</commit_message>
<xml_diff>
--- a/baudrate_calc.xlsx
+++ b/baudrate_calc.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Intended Baudrate</t>
+  </si>
+  <si>
+    <t>Actual Baudrate</t>
+  </si>
+  <si>
+    <t>Clock Frequency (MHz)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,19 +61,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="9"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +127,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +162,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +370,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>115200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <f>((B1*1000000)/B2)</f>
+        <v>868.05555555555554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <f xml:space="preserve"> (B1 * 1000000) / B3</f>
+        <v>115200</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baudrate configuration calculation has been updated.
</commit_message>
<xml_diff>
--- a/baudrate_calc.xlsx
+++ b/baudrate_calc.xlsx
@@ -14,25 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Intended Baudrate</t>
+    <t>Clock Frequency (MHz)</t>
   </si>
   <si>
-    <t>Actual Baudrate</t>
+    <t>Calculated Baudrate</t>
   </si>
   <si>
-    <t>Clock Frequency (MHz)</t>
+    <t>Sample Rate</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Config State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +43,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -57,22 +74,224 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="9"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D749"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D749"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D749"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF61D749"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00CC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CC33"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF61D749"/>
+      <color rgb="FF00CC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -371,50 +590,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>115200</v>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <f>((B1*1000000)/B2)</f>
-        <v>868.05555555555554</v>
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>868</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <f xml:space="preserve"> (B1 * 1000000) / B3</f>
-        <v>115200</v>
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <f>B1*1000000/B3</f>
+        <v>115207.3732718894</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f>IF(B2&lt;B3,"CONFIG OK", "CONFIG ERROR!")</f>
+        <v>CONFIG OK</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$B$2&gt;$B$3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$B$3&gt;=$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>